<commit_message>
generování rasterů l8, ndvi, srtm
</commit_message>
<xml_diff>
--- a/gee_datasets/gee-pouzite-datasety.xlsx
+++ b/gee_datasets/gee-pouzite-datasety.xlsx
@@ -88,6 +88,9 @@
     <t xml:space="preserve">WorldClim BIO Variables V1</t>
   </si>
   <si>
+    <t xml:space="preserve">image</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://developers.google.com/earth-engine/datasets/catalog/WORLDCLIM_V1_BIO</t>
   </si>
   <si>
@@ -112,9 +115,6 @@
     <t xml:space="preserve">NASA SRTM Digital Elevation 30m</t>
   </si>
   <si>
-    <t xml:space="preserve">image</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://developers.google.com/earth-engine/datasets/catalog/USGS_SRTMGL1_003</t>
   </si>
   <si>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">corine</t>
   </si>
   <si>
-    <t xml:space="preserve">COPERNICUS/CORINE/V20/100m</t>
+    <t xml:space="preserve">COPERNICUS/CORINE/V20/100m/2018</t>
   </si>
   <si>
     <t xml:space="preserve">Copernicus CORINE Land Cover</t>
@@ -323,7 +323,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -412,37 +412,37 @@
         <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>31</v>
@@ -474,7 +474,7 @@
         <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
přesun do /export , zjednodušení (odělení funkcí)
</commit_message>
<xml_diff>
--- a/gee_datasets/gee-pouzite-datasety.xlsx
+++ b/gee_datasets/gee-pouzite-datasety.xlsx
@@ -225,12 +225,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -283,7 +289,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,14 +329,14 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="A1:J5"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.77"/>
@@ -347,28 +353,28 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>